<commit_message>
Added Name and Student Number
</commit_message>
<xml_diff>
--- a/WorkSheet.xlsx
+++ b/WorkSheet.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/97984c6fe860f936/Documents/GitHub/CMPG-223-group-8/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_F25DC773A252ABDACC1048C2899952E85ADE58E4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C93AAF95-CD61-4485-9E4A-EB12776CBB13}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="4605" yWindow="2760" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,16 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>Ian Stolz</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,13 +344,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A3:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>37251244</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add name and stud num
</commit_message>
<xml_diff>
--- a/WorkSheet.xlsx
+++ b/WorkSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\CMPG-223-group-8\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashto\Desktop\CMPG\2022\CMPG223\CMPG-223-group-8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B7B9F0C-7D6D-426E-B2AD-8EAA911F9E64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98E0C84-A837-48FF-89FE-972F612C3906}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Albertus van der Walt</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>Student Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ashton du Plessi </t>
   </si>
 </sst>
 </file>
@@ -351,10 +354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -379,6 +382,14 @@
         <v>37073710</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>34202676</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Name and Student number for Ian Stolz
</commit_message>
<xml_diff>
--- a/WorkSheet.xlsx
+++ b/WorkSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/97984c6fe860f936/Documents/GitHub/CMPG-223-group-8/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_F25DC773A252ABDACC1048C2899952E85ADE58E4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C93AAF95-CD61-4485-9E4A-EB12776CBB13}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{A98E0C84-A837-48FF-89FE-972F612C3906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8FC3F549-F7D9-4E67-A2FE-FA94F9035AA8}"/>
   <bookViews>
     <workbookView xWindow="4605" yWindow="2760" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>Albertus van der Walt</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Student Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ashton du Plessi </t>
+  </si>
   <si>
     <t>Ian Stolz</t>
   </si>
@@ -345,19 +357,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:B3"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B3">
+      <c r="B2">
+        <v>37073710</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>34202676</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
         <v>37251244</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated hours for Ian and Franco
</commit_message>
<xml_diff>
--- a/WorkSheet.xlsx
+++ b/WorkSheet.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CODE\Code\CMPG223\PROJECT\CMPG-223-group-8\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/97984c6fe860f936/Documents/GitHub/CMPG-223-group-8/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FB2DAA-9127-4365-A08E-0BC14FC41384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{10FB2DAA-9127-4365-A08E-0BC14FC41384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59C5C19D-C62B-4032-B2D2-68917CB02024}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Progress Report" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Albertus van der Walt</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t xml:space="preserve">Bernard Swanepoel </t>
+  </si>
+  <si>
+    <t>Hours Worked</t>
+  </si>
+  <si>
+    <t>Franco Burger</t>
   </si>
 </sst>
 </file>
@@ -78,8 +84,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -360,56 +369,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>37073710</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>34202676</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>37251244</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>39909476</v>
+      </c>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1">
+        <v>24904635</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ian and Franco worked on design
Designed the edit reservation and created reports for creating and editing a reservation.
</commit_message>
<xml_diff>
--- a/WorkSheet.xlsx
+++ b/WorkSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/97984c6fe860f936/Documents/GitHub/CMPG-223-group-8/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{10FB2DAA-9127-4365-A08E-0BC14FC41384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE166C6F-CBB2-409F-BEC4-1EE725FCA4DF}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{10FB2DAA-9127-4365-A08E-0BC14FC41384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50B458E8-A302-4180-921D-7D112875EDAF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -375,7 +375,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,7 +430,7 @@
         <v>37251244</v>
       </c>
       <c r="C6" s="1">
-        <v>2</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -458,7 +458,7 @@
         <v>24904635</v>
       </c>
       <c r="C10" s="1">
-        <v>2</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Worked on DB. and fixed errors
</commit_message>
<xml_diff>
--- a/WorkSheet.xlsx
+++ b/WorkSheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\CMPG-223-group-8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{228850A7-B7BB-4F0D-93BD-88F693AB95B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D94C966-F219-46DF-9B63-08E107D3542A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>Albertus van der Walt</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>Jacobus</t>
+  </si>
+  <si>
+    <t>1.5 on 09/04</t>
   </si>
 </sst>
 </file>
@@ -402,7 +405,7 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,7 +444,9 @@
       <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="3"/>
+      <c r="F2" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>

</xml_diff>

<commit_message>
Worked on admin UI
Maintain Roles
Maintain Employee
Maintain Room
uwu

Co-Authored-By: AlphaStrategist <111887906+AlphaStrategist@users.noreply.github.com>
Co-Authored-By: Albertus Van der Walt <65769522+naughty00shortie@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/WorkSheet.xlsx
+++ b/WorkSheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\CMPG-223-group-8\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/97984c6fe860f936/Documents/GitHub/CMPG-223-group-8/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D902801-C7D4-423A-9C02-DC54F7107E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{1D902801-C7D4-423A-9C02-DC54F7107E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9635234C-4DC8-4125-8D29-8BBB608AFD0F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress Report" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>Albertus van der Walt</t>
   </si>
@@ -76,6 +76,15 @@
   </si>
   <si>
     <t>1.5 on 09/05</t>
+  </si>
+  <si>
+    <t>2.5 on 09/07</t>
+  </si>
+  <si>
+    <t>2 on 09/07</t>
+  </si>
+  <si>
+    <t>1 on 09/07</t>
   </si>
 </sst>
 </file>
@@ -402,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I7:I8"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,7 +424,8 @@
     <col min="3" max="3" width="19.28515625" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" customWidth="1"/>
     <col min="5" max="6" width="16.42578125" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -425,6 +435,7 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
+      <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -448,24 +459,26 @@
       <c r="G2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
+      <c r="H2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
@@ -485,26 +498,26 @@
       <c r="E4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
     </row>
@@ -527,25 +540,27 @@
       <c r="F6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
+      <c r="G6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
     </row>
@@ -565,26 +580,28 @@
       <c r="E8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
+      <c r="F8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
     </row>
@@ -604,25 +621,28 @@
       <c r="E10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
+      <c r="F10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
     </row>
@@ -639,15 +659,63 @@
       <c r="D12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
worked on backend Admin forms
Co-Authored-By: Ashtondup <110251385+Ashtondup@users.noreply.github.com>
Co-Authored-By: Kajobus <111887945+Kajobus@users.noreply.github.com>
Co-Authored-By: Bernard Swanepoel <104361159+XoXoTheFrozenFox@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/WorkSheet.xlsx
+++ b/WorkSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\CMPG-223-group-8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3526FF-8470-47F3-A52D-633389A61A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC8AA7A-6C83-4DE5-9E3B-D048AC89EF9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-30" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress Report" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
   <si>
     <t>Albertus van der Walt</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>1 on 09/08</t>
+  </si>
+  <si>
+    <t>1 on 09/09</t>
+  </si>
+  <si>
+    <t>1 on 09/10</t>
   </si>
 </sst>
 </file>
@@ -420,7 +426,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,6 +439,7 @@
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
     <col min="8" max="8" width="16.42578125" customWidth="1"/>
     <col min="9" max="9" width="13.42578125" customWidth="1"/>
+    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -472,8 +479,12 @@
       <c r="I2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="J2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
@@ -507,7 +518,9 @@
       <c r="E4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -555,7 +568,9 @@
       <c r="H6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="2"/>
+      <c r="I6" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="3"/>
@@ -594,7 +609,9 @@
       <c r="F8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="H8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -633,7 +650,9 @@
       <c r="F10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="H10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -666,7 +685,9 @@
       <c r="D12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>

</xml_diff>

<commit_message>
added squirrel from npm
</commit_message>
<xml_diff>
--- a/WorkSheet.xlsx
+++ b/WorkSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\CMPG-223-group-8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC8AA7A-6C83-4DE5-9E3B-D048AC89EF9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{172ABCB2-262A-4D69-8924-E660A3F177C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-30" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3315" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Progress Report" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
   <si>
     <t>Albertus van der Walt</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>1 on 09/10</t>
+  </si>
+  <si>
+    <t>2.5 on 09/11</t>
   </si>
 </sst>
 </file>
@@ -425,8 +428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,8 +441,8 @@
     <col min="5" max="6" width="16.42578125" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
     <col min="8" max="8" width="16.42578125" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" customWidth="1"/>
-    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -485,7 +488,9 @@
       <c r="K2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="3"/>
+      <c r="L2" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="M2" s="3"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>